<commit_message>
implement some changes in the inventory route
</commit_message>
<xml_diff>
--- a/client/public/temp.xlsx
+++ b/client/public/temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\tuts\Next\gruspayinventory\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696F34EC-5689-471A-9C39-35620E13FB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AC0C7E-7EF3-42C9-B9AB-BE61C2120881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2270102F-4478-41AE-B238-AABD45A1DA8D}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:AC103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="13.8"/>
@@ -888,9 +888,7 @@
       <c r="K4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="26">
-        <v>45629</v>
-      </c>
+      <c r="L4" s="26"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -941,9 +939,7 @@
       <c r="K5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="26">
-        <v>45630</v>
-      </c>
+      <c r="L5" s="26"/>
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="1:29" ht="14.4">
@@ -978,9 +974,7 @@
       <c r="K6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="26">
-        <v>45631</v>
-      </c>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:29" ht="14.4">
       <c r="B7" s="13"/>

</xml_diff>